<commit_message>
novo design de cards (dados estáticos, depois vou adicionar o js)
</commit_message>
<xml_diff>
--- a/assets/data/arquivos iniciais/2025.06.23___TCE_Plano_de_Acao_SCCG_Restos_a_Pagar (3).xlsx
+++ b/assets/data/arquivos iniciais/2025.06.23___TCE_Plano_de_Acao_SCCG_Restos_a_Pagar (3).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sefazmg-my.sharepoint.com/personal/adriane_paula_fazenda_mg_gov_br/Documents/Área de Trabalho/Planos de Ação - GTS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sefazmg-my.sharepoint.com/personal/pedro_cardoso_fazenda_mg_gov_br/Documents/Documentos/planos_acao/assets/data/arquivos iniciais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82AB8EA4-E0F2-4AEF-883A-F9301CF8C0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{82AB8EA4-E0F2-4AEF-883A-F9301CF8C0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AD852A1-AC3C-4C23-A9C9-60FEAEC2B05F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F3EEB567-1258-4056-8B39-5E0EAA81CA8F}"/>
+    <workbookView xWindow="-16320" yWindow="-1230" windowWidth="16440" windowHeight="28320" xr2:uid="{F3EEB567-1258-4056-8B39-5E0EAA81CA8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de ação - RP" sheetId="1" r:id="rId1"/>
@@ -228,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,6 +259,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -588,7 +597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EAB3268-2C83-4FB5-8BFF-C059DC7D9E96}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -597,7 +608,7 @@
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="69.85546875" customWidth="1"/>
+    <col min="7" max="7" width="50.5703125" style="13" customWidth="1"/>
     <col min="8" max="8" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -608,13 +619,13 @@
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -623,13 +634,13 @@
       <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -638,13 +649,13 @@
       <c r="B3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -653,13 +664,13 @@
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -668,13 +679,13 @@
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -683,13 +694,13 @@
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
@@ -697,7 +708,7 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
@@ -715,7 +726,7 @@
       <c r="F8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -755,7 +766,7 @@
       <c r="F10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
@@ -841,38 +852,38 @@
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
     </row>
     <row r="17" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>1</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
     </row>
     <row r="18" spans="2:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>2</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>